<commit_message>
Updated the first homework of the second term distribution file
</commit_message>
<xml_diff>
--- a/src/Homeworks/Разпределение на задачите за първата домашна работа за втория срок.xlsx
+++ b/src/Homeworks/Разпределение на задачите за първата домашна работа за втория срок.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Development\.NET\Practical-Software-Development-11D\src\Homeworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DD4CFA-076B-43B2-9974-091CE248BA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3311F8-B770-44B1-80BD-4F2428948473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>№ в клас</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>№ Задача - Заявки, включващи външни съединения и/или подзаявки</t>
-  </si>
-  <si>
-    <t>№ Задача -  Заявки, включващи обобщаващи функции (като SUM, COUNT, AVG, MIN, MAX)</t>
   </si>
   <si>
     <t>Може да намерите намерите кода за създаване на базата и нейната документация: https://github.com/plamenna-petrova/Practical-Software-Development-11D/tree/master/src/Exercises/Connecting-Applications-To-Databases/MoviesDatabase</t>
@@ -149,13 +146,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD53DB6B-361E-4167-A1F9-5017E0A722F4}" name="Table2" displayName="Table2" ref="A1:F14" totalsRowShown="0">
-  <autoFilter ref="A1:F14" xr:uid="{FD53DB6B-361E-4167-A1F9-5017E0A722F4}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FD53DB6B-361E-4167-A1F9-5017E0A722F4}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0">
+  <autoFilter ref="A1:E14" xr:uid="{FD53DB6B-361E-4167-A1F9-5017E0A722F4}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3F9678DE-53D9-430B-B660-04FB96A38A42}" name="№ в клас"/>
     <tableColumn id="2" xr3:uid="{8910594E-FF29-489C-B2B7-333D6998A847}" name="Име"/>
     <tableColumn id="3" xr3:uid="{5716F411-613E-49D8-B726-23787206D90D}" name="№ Задача - Заявки към повече от една релации"/>
-    <tableColumn id="4" xr3:uid="{E7AD0A3C-44E8-4637-BD2B-5FBAC86B4FA7}" name="№ Задача -  Заявки, включващи обобщаващи функции (като SUM, COUNT, AVG, MIN, MAX)"/>
     <tableColumn id="5" xr3:uid="{35AE889D-E472-4C2A-B8B8-8BB8F27AEEA8}" name="№ Задача - Заявки, включващи GROUP BY, HAVING"/>
     <tableColumn id="6" xr3:uid="{C9AD348D-75F5-499D-BFB6-0EB366E88575}" name="№ Задача - Заявки, включващи външни съединения и/или подзаявки"/>
   </tableColumns>
@@ -426,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,11 +434,11 @@
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
     <col min="4" max="4" width="83.5546875" customWidth="1"/>
-    <col min="5" max="5" width="47.5546875" customWidth="1"/>
+    <col min="5" max="5" width="69.33203125" customWidth="1"/>
     <col min="6" max="6" width="65.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,137 +449,251 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>